<commit_message>
Added Ethan's progress report.
</commit_message>
<xml_diff>
--- a/ProgressReports/EthanRaymond_ProgressReport.xlsx
+++ b/ProgressReports/EthanRaymond_ProgressReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanraymond/Penn State University/Semester VIII/CMPSC 431W/Semester Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanraymond/Penn State University/Semester VIII/CMPSC 431W/Semester Project/Project.git/ProgressReports/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -570,7 +570,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -637,9 +637,16 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
+      <c r="A6" s="12">
+        <v>42771</v>
+      </c>
+      <c r="B6" s="14">
+        <f>0.3</f>
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>

</xml_diff>